<commit_message>
Bug fix: transform_sqrt to be the same everywhere
</commit_message>
<xml_diff>
--- a/experiments/ac.xlsx
+++ b/experiments/ac.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>pix_per_cell</t>
   </si>
@@ -147,6 +147,51 @@
   </si>
   <si>
     <t>0.9656</t>
+  </si>
+  <si>
+    <t>ac_small</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>re</t>
+  </si>
+  <si>
+    <t>0.9257</t>
+  </si>
+  <si>
+    <t>0.9259</t>
+  </si>
+  <si>
+    <t>0.9505</t>
+  </si>
+  <si>
+    <t>0.9508</t>
+  </si>
+  <si>
+    <t>0.9511</t>
+  </si>
+  <si>
+    <t>0.9662</t>
+  </si>
+  <si>
+    <t>0.9664</t>
+  </si>
+  <si>
+    <t>0.9663</t>
+  </si>
+  <si>
+    <t>0.9513</t>
+  </si>
+  <si>
+    <t>0.9517</t>
+  </si>
+  <si>
+    <t>0.9519</t>
+  </si>
+  <si>
+    <t>0.9634</t>
   </si>
 </sst>
 </file>
@@ -528,22 +573,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -557,31 +602,40 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -597,109 +651,145 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2">
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2">
         <v>5292</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3">
+      <c r="N2" s="3">
         <v>8</v>
       </c>
-      <c r="M2" s="3">
+      <c r="O2" s="3">
         <v>2</v>
       </c>
-      <c r="N2" s="3">
+      <c r="P2" s="3">
         <v>9</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="S2" s="3">
         <v>5292</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="L3">
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3">
         <v>4</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="S3" s="1">
         <v>24300</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="L4">
+      <c r="G4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4">
         <v>16</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>972</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="L5">
+      <c r="G5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5">
         <v>8</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>3</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>8748</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="L6">
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="N6">
         <v>8</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>1728</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -711,37 +801,39 @@
         <v>16</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="L7">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="N7">
         <v>8</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>10</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="S7" s="1">
         <v>5880</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L8">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N8">
         <v>8</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>2</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="S8" s="1">
         <v>6468</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -749,11 +841,13 @@
         <v>18</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="1">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1">
         <v>1764</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -761,8 +855,10 @@
         <v>20</v>
       </c>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -770,26 +866,28 @@
         <v>22</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="K11" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="M11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>6</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>7</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>37</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -797,26 +895,28 @@
         <v>24</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="K12">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="M12">
         <v>2</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="1">
+      <c r="O12" s="1">
         <v>5304</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>2</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="S12" s="1">
         <v>5298</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -824,26 +924,28 @@
         <v>5</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="K13">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="M13">
         <v>4</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="1">
+      <c r="O13" s="1">
         <v>5340</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>4</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="S13" s="1">
         <v>5304</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -851,46 +953,48 @@
         <v>27</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="K14">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="M14">
         <v>8</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="1">
+      <c r="O14" s="1">
         <v>5484</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>8</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="S14" s="1">
         <v>5316</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M15">
         <v>16</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="1">
+      <c r="O15" s="1">
         <v>6060</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>16</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="S15" s="1">
         <v>5340</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -898,51 +1002,53 @@
         <v>29</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16">
         <v>3528</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>32</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="1">
+      <c r="O16" s="1">
         <v>8364</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>32</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="S16" s="1">
         <v>5388</v>
       </c>
     </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="1">
+      <c r="J17" s="1">
         <v>3528</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>64</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="1">
+      <c r="O17" s="1">
         <v>17580</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>64</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="S17" s="1">
         <v>5484</v>
       </c>
     </row>

</xml_diff>